<commit_message>
Add assembly and operations instructions
</commit_message>
<xml_diff>
--- a/Hardware/v3/SMTracker/SMTrackerBOM.xlsx
+++ b/Hardware/v3/SMTracker/SMTrackerBOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mat\Desktop\Final SMorder package\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jakal\Documents\GitHub\OSR_GPS_Collar\Hardware\v3\SMTracker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CD78DCBB-6BCD-4BAA-8F10-DE8F78EF1C39}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5504014B-2479-4A0F-9573-8796F27B5904}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2730" yWindow="1665" windowWidth="20415" windowHeight="14535" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SMTrackerBOM" sheetId="1" r:id="rId1"/>
@@ -93,9 +93,6 @@
     <t>ISP</t>
   </si>
   <si>
-    <t>-</t>
-  </si>
-  <si>
     <t>J1</t>
   </si>
   <si>
@@ -205,17 +202,32 @@
   </si>
   <si>
     <t>https://www.digikey.com/product-detail/en/nexperia-usa-inc/BSH103-215/1727-4319-1-ND/2209929</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/molex/0015910060/WM17457-ND/614773</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF444444"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -235,16 +247,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -461,7 +477,7 @@
   <dimension ref="A1:D999"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -507,13 +523,13 @@
         <v>7</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C3" s="1">
+        <v>1</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>56</v>
-      </c>
-      <c r="C3" s="1">
-        <v>1</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="14.25" x14ac:dyDescent="0.2">
@@ -535,13 +551,13 @@
         <v>9</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C5" s="1">
+        <v>1</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>56</v>
-      </c>
-      <c r="C5" s="1">
-        <v>1</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="14.25" x14ac:dyDescent="0.2">
@@ -563,13 +579,13 @@
         <v>11</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C7" s="1">
+        <v>1</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>56</v>
-      </c>
-      <c r="C7" s="1">
-        <v>1</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="14.25" x14ac:dyDescent="0.2">
@@ -618,69 +634,75 @@
       <c r="A11" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>22</v>
+      <c r="B11" s="2">
+        <v>15910060</v>
+      </c>
+      <c r="C11" s="1">
+        <v>1</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="C12" s="1">
+        <v>1</v>
+      </c>
+      <c r="D12" s="1" t="s">
         <v>24</v>
-      </c>
-      <c r="C12" s="1">
-        <v>1</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B13" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C13" s="1">
+        <v>1</v>
+      </c>
+      <c r="D13" s="1" t="s">
         <v>24</v>
-      </c>
-      <c r="C13" s="1">
-        <v>1</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="C14" s="1">
+        <v>1</v>
+      </c>
+      <c r="D14" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="C14" s="1">
-        <v>1</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="C15" s="1">
+        <v>1</v>
+      </c>
+      <c r="D15" s="1" t="s">
         <v>31</v>
-      </c>
-      <c r="C15" s="1">
-        <v>1</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>16</v>
@@ -694,133 +716,133 @@
     </row>
     <row r="17" spans="1:4" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B17" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="C17" s="1">
+        <v>1</v>
+      </c>
+      <c r="D17" s="1" t="s">
         <v>35</v>
-      </c>
-      <c r="C17" s="1">
-        <v>1</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B18" s="1" t="s">
-        <v>38</v>
-      </c>
       <c r="C18" s="1">
         <v>1</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B19" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="C19" s="1">
+        <v>1</v>
+      </c>
+      <c r="D19" s="1" t="s">
         <v>40</v>
-      </c>
-      <c r="C19" s="1">
-        <v>1</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B20" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="C20" s="1">
+        <v>1</v>
+      </c>
+      <c r="D20" s="1" t="s">
         <v>43</v>
-      </c>
-      <c r="C20" s="1">
-        <v>1</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B21" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C21" s="1">
+        <v>1</v>
+      </c>
+      <c r="D21" s="1" t="s">
         <v>43</v>
-      </c>
-      <c r="C21" s="1">
-        <v>1</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B22" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B22" s="1" t="s">
-        <v>47</v>
-      </c>
       <c r="C22" s="1">
         <v>1</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B23" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C23" s="1">
+        <v>1</v>
+      </c>
+      <c r="D23" s="1" t="s">
         <v>40</v>
-      </c>
-      <c r="C23" s="1">
-        <v>1</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B24" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="C24" s="1">
+        <v>1</v>
+      </c>
+      <c r="D24" s="1" t="s">
         <v>50</v>
-      </c>
-      <c r="C24" s="1">
-        <v>1</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B25" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="C25" s="1">
+        <v>1</v>
+      </c>
+      <c r="D25" s="1" t="s">
         <v>53</v>
-      </c>
-      <c r="C25" s="1">
-        <v>1</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B26" s="1">
         <v>473521001</v>
@@ -829,7 +851,7 @@
         <v>1</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1821,8 +1843,9 @@
     <hyperlink ref="D20" r:id="rId12" xr:uid="{4D889B3C-4067-47CF-9252-30F342C5C0D4}"/>
     <hyperlink ref="D22" r:id="rId13" xr:uid="{8EC8837E-A6E7-48A8-9981-465BC0B24DA7}"/>
     <hyperlink ref="D25" r:id="rId14" xr:uid="{A113DEE1-D7CA-40A7-B125-38AB970C8B99}"/>
+    <hyperlink ref="D11" r:id="rId15" xr:uid="{ADBB7CBA-F38D-45D4-9038-8F892D00002D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup orientation="portrait" r:id="rId15"/>
+  <pageSetup orientation="portrait" r:id="rId16"/>
 </worksheet>
 </file>
</xml_diff>